<commit_message>
update Schedule and Design document
</commit_message>
<xml_diff>
--- a/doc/04.Schedule/工作计划.xlsx
+++ b/doc/04.Schedule/工作计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AT$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$48</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="168">
   <si>
     <t>提示：点上面加号可以展开计划审核明细</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -460,284 +460,314 @@
     <t>20</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>编制文档</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步平台</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>编制同步平台的具体实现功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>结帐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>结帐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据导入</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据导入</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据核对</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据核对</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统设置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>资金管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(数据月结、日结)设计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>(数据月结、日结)功能开发及相关报表调整</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>程序优化</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>各报表查询速度优化及实现SQL作业脚本每日股票收盘价取得</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器配置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目服务器迁移准备工作，10.10.10.2服务器相关软件安装配置。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Wind数据同步</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1分钟数同步</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步股票的1分钟数据</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>数据核对</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>交割单数据导入，并按账号核对交割单与交易员导入的数据是否完全。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>交易系统实施</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>对零散的同步整合在一个平台下面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报屏系统</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>现有报屏系统优化</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>对帐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>日、周、月 对帐流程说明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>林福生、王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>王海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号、人员、股票 固定格式报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员、股票、账号 固定格式报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员、账户、股票 多维度查询报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员、账户、股票 多维度查询报表修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票汇总下面能看到交易数据明细</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>李四</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>合计：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员收益情况台帐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以统计某段时间内每天每个人收益明细，及所有人的收益汇总</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>按交割单数据统计账号的收益流水和和相关报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>短差交易员每天买卖标识用程序实现</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>程序开发</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>三方账号盈亏统计需要重新开发(与现有的数据分开来)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>买卖标识报表上增加 盈亏金额和 多买、多卖股票数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>王贵斌</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>短差交易员每天买卖标识用程序实现</t>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>编制文档</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>同步平台</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>编制同步平台的具体实现功能</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>模块</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>结帐</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>结帐</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>报表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据导入</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据导入</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>报表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据核对</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据核对</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>权限管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>系统设置</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>资金管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(数据月结、日结)设计</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人员</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>(数据月结、日结)功能开发及相关报表调整</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>程序优化</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>各报表查询速度优化及实现SQL作业脚本每日股票收盘价取得</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>服务器配置</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>项目服务器迁移准备工作，10.10.10.2服务器相关软件安装配置。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Wind数据同步</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1分钟数同步</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>同步股票的1分钟数据</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>数据核对</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>交割单数据导入，并按账号核对交割单与交易员导入的数据是否完全。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>交易系统实施</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>对零散的同步整合在一个平台下面</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>报屏系统</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>现有报屏系统优化</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>对帐</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>日、周、月 对帐流程说明</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>林福生、王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>王海</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号、人员、股票 固定格式报表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人员、股票、账号 固定格式报表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人员、账户、股票 多维度查询报表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>报表修改</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人员、账户、股票 多维度查询报表修改</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>股票汇总下面能看到交易数据明细</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人员</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>张三</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>李四</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>合计：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>报表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人员收益情况台帐</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以统计某段时间内每天每个人收益明细，及所有人的收益汇总</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>报表</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>按交割单数据统计账号的收益流水和和相关报表</t>
+    <t>账户信息表增加字段，开户收在地</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1494,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW314"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AV18" sqref="AV18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12" outlineLevelCol="1"/>
@@ -1608,7 +1638,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>4</v>
@@ -1623,7 +1653,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="14" t="s">
@@ -1742,7 +1772,7 @@
         <v>68</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F3" s="53" t="s">
         <v>47</v>
@@ -1776,7 +1806,7 @@
         <v>68</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>76</v>
@@ -1808,7 +1838,7 @@
         <v>69</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>66</v>
@@ -1842,7 +1872,7 @@
         <v>69</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>64</v>
@@ -1876,7 +1906,7 @@
         <v>68</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>79</v>
@@ -1908,10 +1938,10 @@
         <v>68</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="58">
@@ -1940,7 +1970,7 @@
         <v>68</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>73</v>
@@ -2007,10 +2037,10 @@
         <v>68</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="58">
@@ -2039,10 +2069,10 @@
         <v>68</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G11" s="26"/>
       <c r="H11" s="58">
@@ -2068,13 +2098,13 @@
         <v>46</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E12" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="58">
@@ -2084,7 +2114,7 @@
         <v>42623</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
@@ -2103,10 +2133,10 @@
         <v>68</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="58">
@@ -2116,7 +2146,7 @@
         <v>42624</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
@@ -2135,7 +2165,7 @@
         <v>68</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F14" s="25" t="s">
         <v>80</v>
@@ -2167,7 +2197,7 @@
         <v>68</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F15" s="25" t="s">
         <v>78</v>
@@ -2199,7 +2229,7 @@
         <v>69</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" s="55" t="s">
         <v>57</v>
@@ -2259,13 +2289,13 @@
         <v>46</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="56">
@@ -2273,7 +2303,7 @@
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
@@ -2289,13 +2319,13 @@
         <v>46</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G18" s="26"/>
       <c r="H18" s="56">
@@ -2303,7 +2333,7 @@
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
@@ -2319,13 +2349,13 @@
         <v>46</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G19" s="26"/>
       <c r="H19" s="56">
@@ -2333,7 +2363,7 @@
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
@@ -2352,7 +2382,7 @@
         <v>69</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F20" s="55" t="s">
         <v>58</v>
@@ -2382,10 +2412,10 @@
         <v>68</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F21" s="55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G21" s="26"/>
       <c r="H21" s="56">
@@ -2412,10 +2442,10 @@
         <v>69</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F22" s="55" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="G22" s="26"/>
       <c r="H22" s="56">
@@ -2423,14 +2453,14 @@
       </c>
       <c r="I22" s="27"/>
       <c r="J22" s="24" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
     </row>
     <row r="23" spans="1:12" ht="25.15" customHeight="1">
       <c r="A23" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="33" t="s">
         <v>44</v>
@@ -2442,10 +2472,10 @@
         <v>68</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F23" s="55" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G23" s="26"/>
       <c r="H23" s="56">
@@ -2453,14 +2483,14 @@
       </c>
       <c r="I23" s="27"/>
       <c r="J23" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
     </row>
     <row r="24" spans="1:12" ht="25.15" customHeight="1">
       <c r="A24" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B24" s="33" t="s">
         <v>44</v>
@@ -2472,10 +2502,10 @@
         <v>68</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F24" s="55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G24" s="26"/>
       <c r="H24" s="61">
@@ -2490,7 +2520,7 @@
     </row>
     <row r="25" spans="1:12" ht="25.15" customHeight="1">
       <c r="A25" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" s="33" t="s">
         <v>44</v>
@@ -2502,10 +2532,10 @@
         <v>68</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F25" s="55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="62"/>
@@ -2518,7 +2548,7 @@
     </row>
     <row r="26" spans="1:12" ht="25.15" customHeight="1">
       <c r="A26" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B26" s="33" t="s">
         <v>44</v>
@@ -2530,13 +2560,13 @@
         <v>68</v>
       </c>
       <c r="E26" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="26" t="s">
         <v>140</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>141</v>
-      </c>
-      <c r="G26" s="26" t="s">
-        <v>142</v>
       </c>
       <c r="H26" s="56">
         <v>42660</v>
@@ -2550,7 +2580,7 @@
     </row>
     <row r="27" spans="1:12" ht="29.25" customHeight="1">
       <c r="A27" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B27" s="33" t="s">
         <v>44</v>
@@ -2562,13 +2592,13 @@
         <v>68</v>
       </c>
       <c r="E27" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" s="26" t="s">
         <v>147</v>
-      </c>
-      <c r="F27" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="H27" s="56">
         <v>42663</v>
@@ -2582,7 +2612,7 @@
     </row>
     <row r="28" spans="1:12" ht="25.15" customHeight="1">
       <c r="A28" s="23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B28" s="33" t="s">
         <v>44</v>
@@ -2594,7 +2624,7 @@
         <v>69</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F28" s="25" t="s">
         <v>59</v>
@@ -2614,7 +2644,7 @@
     </row>
     <row r="29" spans="1:12" ht="25.15" customHeight="1">
       <c r="A29" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B29" s="33" t="s">
         <v>44</v>
@@ -2626,10 +2656,10 @@
         <v>69</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G29" s="26"/>
       <c r="H29" s="56">
@@ -2637,14 +2667,14 @@
       </c>
       <c r="I29" s="27"/>
       <c r="J29" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
     </row>
     <row r="30" spans="1:12" ht="25.15" customHeight="1">
       <c r="A30" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B30" s="33" t="s">
         <v>44</v>
@@ -2656,10 +2686,10 @@
         <v>69</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G30" s="26"/>
       <c r="H30" s="56">
@@ -2674,7 +2704,7 @@
     </row>
     <row r="31" spans="1:12" ht="25.15" customHeight="1">
       <c r="A31" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B31" s="33" t="s">
         <v>44</v>
@@ -2686,7 +2716,7 @@
         <v>69</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>52</v>
@@ -2697,14 +2727,14 @@
       </c>
       <c r="I31" s="27"/>
       <c r="J31" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:12" ht="25.15" customHeight="1">
       <c r="A32" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B32" s="33" t="s">
         <v>44</v>
@@ -2716,7 +2746,7 @@
         <v>69</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>50</v>
@@ -2734,7 +2764,7 @@
     </row>
     <row r="33" spans="1:49" ht="25.15" customHeight="1">
       <c r="A33" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B33" s="33" t="s">
         <v>44</v>
@@ -2746,7 +2776,7 @@
         <v>69</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>54</v>
@@ -2764,7 +2794,7 @@
     </row>
     <row r="34" spans="1:49" ht="25.15" customHeight="1">
       <c r="A34" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B34" s="33" t="s">
         <v>44</v>
@@ -2776,7 +2806,7 @@
         <v>69</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" s="55" t="s">
         <v>55</v>
@@ -2792,7 +2822,7 @@
     </row>
     <row r="35" spans="1:49" ht="25.15" customHeight="1">
       <c r="A35" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B35" s="33" t="s">
         <v>44</v>
@@ -2804,7 +2834,7 @@
         <v>69</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F35" s="25" t="s">
         <v>61</v>
@@ -2820,7 +2850,7 @@
     </row>
     <row r="36" spans="1:49" ht="27.75" customHeight="1">
       <c r="A36" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B36" s="33" t="s">
         <v>44</v>
@@ -2832,7 +2862,7 @@
         <v>69</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F36" s="25" t="s">
         <v>62</v>
@@ -2850,7 +2880,7 @@
     </row>
     <row r="37" spans="1:49" ht="25.15" customHeight="1">
       <c r="A37" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B37" s="33" t="s">
         <v>44</v>
@@ -2862,7 +2892,7 @@
         <v>69</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F37" s="55" t="s">
         <v>53</v>
@@ -2877,44 +2907,86 @@
       <c r="L37" s="24"/>
     </row>
     <row r="38" spans="1:49" ht="25.15" customHeight="1">
-      <c r="A38" s="23"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="25"/>
+      <c r="A38" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>160</v>
+      </c>
       <c r="G38" s="26"/>
       <c r="H38" s="56"/>
       <c r="I38" s="27"/>
-      <c r="J38" s="24"/>
+      <c r="J38" s="24" t="s">
+        <v>71</v>
+      </c>
       <c r="K38" s="24"/>
       <c r="L38" s="24"/>
     </row>
     <row r="39" spans="1:49" ht="25.15" customHeight="1">
-      <c r="A39" s="23"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="25"/>
+      <c r="A39" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="G39" s="26"/>
-      <c r="H39" s="27"/>
+      <c r="H39" s="56"/>
       <c r="I39" s="27"/>
-      <c r="J39" s="24"/>
+      <c r="J39" s="24" t="s">
+        <v>163</v>
+      </c>
       <c r="K39" s="24"/>
       <c r="L39" s="24"/>
     </row>
     <row r="40" spans="1:49" ht="25.15" customHeight="1">
-      <c r="A40" s="23"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="25"/>
+      <c r="A40" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>167</v>
+      </c>
       <c r="G40" s="26"/>
       <c r="H40" s="27"/>
       <c r="I40" s="27"/>
-      <c r="J40" s="24"/>
+      <c r="J40" s="24" t="s">
+        <v>71</v>
+      </c>
       <c r="K40" s="24"/>
       <c r="L40" s="24"/>
     </row>
@@ -15048,7 +15120,7 @@
       <c r="D1" s="50"/>
       <c r="E1" s="51"/>
       <c r="F1" s="57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -15069,7 +15141,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>4</v>
@@ -15084,7 +15156,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21" customHeight="1">
@@ -15106,7 +15178,7 @@
       <c r="H3" s="58"/>
       <c r="I3" s="56"/>
       <c r="J3" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1">
@@ -15128,7 +15200,7 @@
       <c r="H4" s="58"/>
       <c r="I4" s="56"/>
       <c r="J4" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -15150,7 +15222,7 @@
   <sheetData>
     <row r="3" spans="2:11">
       <c r="B3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="60">
         <v>42370</v>
@@ -15182,7 +15254,7 @@
     </row>
     <row r="4" spans="2:11">
       <c r="B4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4">
         <v>1000</v>
@@ -15214,7 +15286,7 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5">
         <v>678</v>
@@ -15246,7 +15318,7 @@
     </row>
     <row r="6" spans="2:11">
       <c r="B6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6">
         <f>SUM(C4:C5)</f>

</xml_diff>